<commit_message>
add skeleton for chapter 4 pick&place
</commit_message>
<xml_diff>
--- a/content/pick-n-place-project/set-plc-module-parameters/docs/Pick&Placer_PLCTags.de.xlsx
+++ b/content/pick-n-place-project/set-plc-module-parameters/docs/Pick&Placer_PLCTags.de.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLC Tags" sheetId="1" r:id="R021266c21ee74e33"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Constants" sheetId="2" r:id="R1209eb64f6c64842"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TagTable Properties" sheetId="3" r:id="R40069e9551e74d0f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PLC Tags" sheetId="1" r:id="R0c86b3d086554ae6"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Constants" sheetId="2" r:id="Ra75f122787914766"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TagTable Properties" sheetId="3" r:id="R89afdb79eee84a47"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="216">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="219">
   <x:si>
     <x:t xml:space="preserve">Name</x:t>
   </x:si>
@@ -264,7 +264,7 @@
     <x:t xml:space="preserve">%E0.1</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Transportband Werkstück am Bandanfang (100XD1)</x:t>
+    <x:t xml:space="preserve">Transportband Werkstück am Bandanfang (100BG1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PPTR_BG_PartAtSep</x:t>
@@ -273,7 +273,7 @@
     <x:t xml:space="preserve">%E0.2</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Transportband Werkstück am Vereinzeler (100XD1)</x:t>
+    <x:t xml:space="preserve">Transportband Werkstück am Vereinzeler (100BG2)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PPTR_BG_BackupPart</x:t>
@@ -282,7 +282,7 @@
     <x:t xml:space="preserve">%E0.3</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Transportband Werkstück beim Bandende (100XD1)</x:t>
+    <x:t xml:space="preserve">Transportband Werkstück beim Bandende (100BG3)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_BG_CarrierRetracted</x:t>
@@ -291,7 +291,7 @@
     <x:t xml:space="preserve">%E0.4</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Schlitten eingefahren (120XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Schlitten eingefahren (120BG1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_BG_CarrierExtended</x:t>
@@ -300,7 +300,7 @@
     <x:t xml:space="preserve">%E0.5</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Schlitten ausgefahren (120XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Schlitten ausgefahren (120BG2)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_BG_SuctTop</x:t>
@@ -309,7 +309,7 @@
     <x:t xml:space="preserve">%E0.6</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Sauger oben (120XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Sauger oben (120BG3)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_BP_PartSuckedOn</x:t>
@@ -318,7 +318,7 @@
     <x:t xml:space="preserve">%E0.7</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Werkstück angesaugt (120XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Werkstück angesaugt (120PB4)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_Pa_SF_Reset</x:t>
@@ -327,7 +327,7 @@
     <x:t xml:space="preserve">%E1.0</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Reset (160XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Reset (160SF2)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_Pa_SF_Start</x:t>
@@ -336,7 +336,7 @@
     <x:t xml:space="preserve">%E1.1</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Start (160XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Start (160SF3)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_Pa_SF_Stop</x:t>
@@ -345,7 +345,7 @@
     <x:t xml:space="preserve">%E1.2</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Stop (160XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Stop (160SF4)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_Pa_SF_ManAuto</x:t>
@@ -354,7 +354,7 @@
     <x:t xml:space="preserve">%E1.3</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Manual - Auto (160XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Manual - Auto (160SF5)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">CC_Spare_I1.4</x:t>
@@ -390,7 +390,7 @@
     <x:t xml:space="preserve">%A0.0</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Transportband Vereinzeler ausfahren (100XD1)</x:t>
+    <x:t xml:space="preserve">Transportband Vereinzeler ausfahren (105MB8)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_SC_Green</x:t>
@@ -399,7 +399,7 @@
     <x:t xml:space="preserve">%A0.1</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Turmleuchte grün (130XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Turmleuchte grün (130PF1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_SC_Yellow</x:t>
@@ -408,7 +408,7 @@
     <x:t xml:space="preserve">%A0.2</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Turmleuchte gelb (130XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Turmleuchte gelb (130PF1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_SC_Red</x:t>
@@ -417,7 +417,7 @@
     <x:t xml:space="preserve">%A0.3</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Turmleuchte rot (130XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Turmleuchte rot (130PF1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_MB_CarrierExtend</x:t>
@@ -426,7 +426,7 @@
     <x:t xml:space="preserve">%A0.4</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Schlitten einfahren (125XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Schlitten einfahren (125MB1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_MB_CarrierRetract</x:t>
@@ -435,7 +435,7 @@
     <x:t xml:space="preserve">%A0.5</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Schlitten ausfahren (15XD1.1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Schlitten ausfahren (125MB2)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_MB_SuctDown</x:t>
@@ -444,7 +444,7 @@
     <x:t xml:space="preserve">%A0.6</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Sauger nach unten (15XD1.1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Sauger nach unten (125MB3)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_MB_VacuumOn</x:t>
@@ -453,7 +453,7 @@
     <x:t xml:space="preserve">%A0.7</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Vakuum ein (15XD1.1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Vakuum ein (125MB4)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_Pa_PF_ControlCircuit</x:t>
@@ -462,13 +462,16 @@
     <x:t xml:space="preserve">%A1.0</x:t>
   </x:si>
   <x:si>
+    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle LED Steuerspannung Ein (Reset) (160SF2)</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">PIPL_Pa_PF_Error</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">%A1.1</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Fehler (160XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle LED Fehler (160PF2)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PIPL_Pa_PF_Start</x:t>
@@ -477,6 +480,9 @@
     <x:t xml:space="preserve">%A1.2</x:t>
   </x:si>
   <x:si>
+    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle LED Start (160SF3)</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">CC_Spare_O1.3</x:t>
   </x:si>
   <x:si>
@@ -528,7 +534,7 @@
     <x:t xml:space="preserve">%AW272</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Transportband Bandmotor Geschwindigkeit Option (105XD3)</x:t>
+    <x:t xml:space="preserve">Transportband Bandmotor Geschwindigkeit Option (105TF1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">CC_Spare_OW274</x:t>
@@ -546,7 +552,7 @@
     <x:t xml:space="preserve">%E1000.0</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Not-Halt (160XD1)</x:t>
+    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Not-Halt Channel 1 (160SF1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">CC_Spare_I1000.1</x:t>
@@ -573,6 +579,9 @@
     <x:t xml:space="preserve">%E1000.4</x:t>
   </x:si>
   <x:si>
+    <x:t xml:space="preserve">Pick&amp;Placer Bedienstelle Not-Halt Channel 2 (160SF1)</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">CC_Spare_I1000.5</x:t>
   </x:si>
   <x:si>
@@ -597,7 +606,7 @@
     <x:t xml:space="preserve">%A1050.0</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Freigabe Not-Halt (81KF7)</x:t>
+    <x:t xml:space="preserve">Freigabe Not-Halt Channel 1 (81KF7)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">CC_KF_EStopCh2</x:t>
@@ -606,7 +615,7 @@
     <x:t xml:space="preserve">%A1050.1</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Freigabe Not-Halt (81KF8)</x:t>
+    <x:t xml:space="preserve">Freigabe Not-Halt Channel 2 (81KF8)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PPTR_TF_DriveForward</x:t>
@@ -615,7 +624,7 @@
     <x:t xml:space="preserve">%A1050.2</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Transportband Bandmotor Vorwärts (100XD1)</x:t>
+    <x:t xml:space="preserve">Transportband Bandmotor Vorwärts (105TF1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">PPTR_TF_DriveReverse</x:t>
@@ -624,7 +633,7 @@
     <x:t xml:space="preserve">%A1050.3</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">Transportband Bandmotor Rückwärts (100XD1)</x:t>
+    <x:t xml:space="preserve">Transportband Bandmotor Rückwärts (105TF1)</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">CC_Spare_O1050.4</x:t>
@@ -2197,7 +2206,7 @@
         <x:v>149</x:v>
       </x:c>
       <x:c r="E47" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="F47" s="0" t="s">
         <x:v>15</x:v>
@@ -2217,7 +2226,7 @@
     </x:row>
     <x:row r="48">
       <x:c r="A48" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
         <x:v>79</x:v>
@@ -2226,10 +2235,10 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D48" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="E48" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F48" s="0" t="s">
         <x:v>15</x:v>
@@ -2249,7 +2258,7 @@
     </x:row>
     <x:row r="49">
       <x:c r="A49" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
         <x:v>79</x:v>
@@ -2258,10 +2267,10 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D49" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="E49" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F49" s="0" t="s">
         <x:v>15</x:v>
@@ -2281,7 +2290,7 @@
     </x:row>
     <x:row r="50">
       <x:c r="A50" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
         <x:v>79</x:v>
@@ -2290,7 +2299,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D50" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="E50" s="0" t="s">
         <x:v>117</x:v>
@@ -2313,7 +2322,7 @@
     </x:row>
     <x:row r="51">
       <x:c r="A51" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
         <x:v>79</x:v>
@@ -2322,7 +2331,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D51" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="E51" s="0" t="s">
         <x:v>117</x:v>
@@ -2345,7 +2354,7 @@
     </x:row>
     <x:row r="52">
       <x:c r="A52" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
         <x:v>79</x:v>
@@ -2354,7 +2363,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D52" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="E52" s="0" t="s">
         <x:v>117</x:v>
@@ -2377,7 +2386,7 @@
     </x:row>
     <x:row r="53">
       <x:c r="A53" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
         <x:v>79</x:v>
@@ -2386,7 +2395,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D53" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="E53" s="0" t="s">
         <x:v>117</x:v>
@@ -2409,7 +2418,7 @@
     </x:row>
     <x:row r="54">
       <x:c r="A54" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
         <x:v>79</x:v>
@@ -2418,7 +2427,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D54" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="E54" s="0" t="s">
         <x:v>117</x:v>
@@ -2441,16 +2450,16 @@
     </x:row>
     <x:row r="55">
       <x:c r="A55" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
         <x:v>79</x:v>
       </x:c>
       <x:c r="C55" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D55" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="E55" s="0" t="s">
         <x:v>117</x:v>
@@ -2473,16 +2482,16 @@
     </x:row>
     <x:row r="56">
       <x:c r="A56" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
         <x:v>168</x:v>
       </x:c>
-      <x:c r="B56" s="0" t="s">
-        <x:v>79</x:v>
-      </x:c>
-      <x:c r="C56" s="0" t="s">
-        <x:v>166</x:v>
-      </x:c>
       <x:c r="D56" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="E56" s="0" t="s">
         <x:v>117</x:v>
@@ -2505,19 +2514,19 @@
     </x:row>
     <x:row r="57">
       <x:c r="A57" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
         <x:v>79</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D57" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="E57" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="F57" s="0" t="s">
         <x:v>15</x:v>
@@ -2537,16 +2546,16 @@
     </x:row>
     <x:row r="58">
       <x:c r="A58" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
         <x:v>79</x:v>
       </x:c>
       <x:c r="C58" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D58" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="E58" s="0" t="s">
         <x:v>117</x:v>
@@ -2569,19 +2578,19 @@
     </x:row>
     <x:row r="59">
       <x:c r="A59" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C59" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D59" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="E59" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="F59" s="0" t="s">
         <x:v>15</x:v>
@@ -2601,16 +2610,16 @@
     </x:row>
     <x:row r="60">
       <x:c r="A60" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C60" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D60" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="E60" s="0" t="s">
         <x:v>117</x:v>
@@ -2633,16 +2642,16 @@
     </x:row>
     <x:row r="61">
       <x:c r="A61" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D61" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="E61" s="0" t="s">
         <x:v>117</x:v>
@@ -2665,16 +2674,16 @@
     </x:row>
     <x:row r="62">
       <x:c r="A62" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D62" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="E62" s="0" t="s">
         <x:v>117</x:v>
@@ -2697,19 +2706,19 @@
     </x:row>
     <x:row r="63">
       <x:c r="A63" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D63" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="E63" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="F63" s="0" t="s">
         <x:v>15</x:v>
@@ -2729,16 +2738,16 @@
     </x:row>
     <x:row r="64">
       <x:c r="A64" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D64" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="E64" s="0" t="s">
         <x:v>117</x:v>
@@ -2761,16 +2770,16 @@
     </x:row>
     <x:row r="65">
       <x:c r="A65" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C65" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D65" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="E65" s="0" t="s">
         <x:v>117</x:v>
@@ -2793,16 +2802,16 @@
     </x:row>
     <x:row r="66">
       <x:c r="A66" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C66" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D66" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="E66" s="0" t="s">
         <x:v>117</x:v>
@@ -2825,19 +2834,19 @@
     </x:row>
     <x:row r="67">
       <x:c r="A67" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C67" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D67" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="E67" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="F67" s="0" t="s">
         <x:v>15</x:v>
@@ -2857,19 +2866,19 @@
     </x:row>
     <x:row r="68">
       <x:c r="A68" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D68" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="E68" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F68" s="0" t="s">
         <x:v>15</x:v>
@@ -2889,19 +2898,19 @@
     </x:row>
     <x:row r="69">
       <x:c r="A69" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D69" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="E69" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="F69" s="0" t="s">
         <x:v>15</x:v>
@@ -2921,19 +2930,19 @@
     </x:row>
     <x:row r="70">
       <x:c r="A70" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C70" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D70" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="E70" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="F70" s="0" t="s">
         <x:v>15</x:v>
@@ -2953,16 +2962,16 @@
     </x:row>
     <x:row r="71">
       <x:c r="A71" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C71" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D71" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="E71" s="0" t="s">
         <x:v>117</x:v>
@@ -2985,16 +2994,16 @@
     </x:row>
     <x:row r="72">
       <x:c r="A72" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C72" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D72" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="E72" s="0" t="s">
         <x:v>117</x:v>
@@ -3017,16 +3026,16 @@
     </x:row>
     <x:row r="73">
       <x:c r="A73" s="0" t="s">
-        <x:v>209</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C73" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D73" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="E73" s="0" t="s">
         <x:v>117</x:v>
@@ -3049,16 +3058,16 @@
     </x:row>
     <x:row r="74">
       <x:c r="A74" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C74" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="D74" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="E74" s="0" t="s">
         <x:v>117</x:v>
@@ -3097,7 +3106,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
@@ -3115,10 +3124,10 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>218</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
@@ -3145,7 +3154,7 @@
     </x:row>
     <x:row r="4">
       <x:c r="A4" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
         <x:v>16</x:v>

</xml_diff>